<commit_message>
update test with parent for test 1
</commit_message>
<xml_diff>
--- a/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test2/QuerySet2.xlsx
+++ b/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test2/QuerySet2.xlsx
@@ -4,14 +4,10 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Complex" sheetId="4" r:id="rId1"/>
-    <sheet name="Follows" sheetId="1" r:id="rId2"/>
-    <sheet name="FollowsStar" sheetId="2" r:id="rId3"/>
-    <sheet name="Parent" sheetId="3" r:id="rId4"/>
-    <sheet name="ParentStar" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Index</t>
   </si>
@@ -44,6 +40,9 @@
   </si>
   <si>
     <t>Select s</t>
+  </si>
+  <si>
+    <t>All statements HaveResult</t>
   </si>
 </sst>
 </file>
@@ -59,6 +58,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -93,16 +93,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,65 +390,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3B02F3-8668-4835-B18A-9EFEA275CE21}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="78.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="6" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="76.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="39.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="128" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -454,7 +416,7 @@
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -462,162 +424,39 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="E2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="7"/>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="7"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8A40C96-D5A1-4C6E-8929-672E2B10CBA0}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="47.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{870584E9-F36E-45C6-860B-FA9B6E4871B1}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1D4012-BEAE-42F9-8807-9F5970E9D8C7}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add test case to excel
</commit_message>
<xml_diff>
--- a/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test2/QuerySet2.xlsx
+++ b/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test2/QuerySet2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Index</t>
   </si>
@@ -46,6 +46,132 @@
   </si>
   <si>
     <t>1,10,11,12,13,14,15,16,17,18,19,2,20,21,22,23,24,25,26,27,28,29,3,30,31,32,33,34,35,36,37,38,4,5,6,7,8,9</t>
+  </si>
+  <si>
+    <t>stmt s, s1, s2;</t>
+  </si>
+  <si>
+    <t>Select s with s1.stmt#=s2.stmt#</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym With StmtStmt NoCommonSynonym HaveResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym With StmtStmt CommonSynonym HaveResult</t>
+  </si>
+  <si>
+    <t>Select s1 with s1.stmt#=s2.stmt#</t>
+  </si>
+  <si>
+    <t>stmt s1, s2;</t>
+  </si>
+  <si>
+    <t>Select s with s.stmt#=3</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym With StmtInt CommonSynonym HaveResult</t>
+  </si>
+  <si>
+    <t>Select s1 with s2.stmt#=5</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym With StmtInt NoCommonSynonym HaveResult</t>
+  </si>
+  <si>
+    <t>Select s with s.stmt#="hello"</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym With StmtStr NonCompatible WithType NoResult</t>
+  </si>
+  <si>
+    <t>Select s with s.stmt# = a.stmt#</t>
+  </si>
+  <si>
+    <t>stmt s; assign a;</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym With StmtAssign HaveResult</t>
+  </si>
+  <si>
+    <t>stmt s; while w;</t>
+  </si>
+  <si>
+    <t>Select s with s.stmt# = w.stmt#</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym With StmtWhile HaveResult</t>
+  </si>
+  <si>
+    <t>stmt s; if f;</t>
+  </si>
+  <si>
+    <t>Select s with s.stmt# = f.stmt#</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym With StmtIf HaveResult</t>
+  </si>
+  <si>
+    <t>stmt s; prog_line pl;</t>
+  </si>
+  <si>
+    <t>Select s with s.stmt# = pl</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym With StmtProgLine HaveResult</t>
+  </si>
+  <si>
+    <t>stmt s; call cl;</t>
+  </si>
+  <si>
+    <t>Select s with s.stmt# = cl.stmt#</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym With StmtCall HaveResult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assign a; </t>
+  </si>
+  <si>
+    <t>Select a with a.stmt# = 4</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym With AssignInt HaveResult</t>
+  </si>
+  <si>
+    <t>Select a with a.stmt# = a.stmt#</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym With AssignAssign LhsRhsSame HaveResult</t>
+  </si>
+  <si>
+    <t>assign a1, a2;</t>
+  </si>
+  <si>
+    <t>Select a1 with a1.stmt# = a2.stmt#</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym With AssignAssign CommonSynonym HaveResult</t>
+  </si>
+  <si>
+    <t>assign a, a1, a2;</t>
+  </si>
+  <si>
+    <t>Select a with a1.stmt# = a2.stmt#</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym With AssignAssign NoCommonSynonym HaveResult</t>
+  </si>
+  <si>
+    <t>assign a; while w;</t>
+  </si>
+  <si>
+    <t>Select a with a.stmt#=w.stmt#</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym With AssignWhile NoResult</t>
   </si>
 </sst>
 </file>
@@ -395,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3B02F3-8668-4835-B18A-9EFEA275CE21}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,16 +569,184 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D30" s="7"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D31" s="7"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D32" s="7"/>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated excel file to allow collaboration
</commit_message>
<xml_diff>
--- a/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test2/QuerySet2.xlsx
+++ b/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test2/QuerySet2.xlsx
@@ -4,10 +4,15 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="4" r:id="rId1"/>
+    <sheet name="Andy" sheetId="5" r:id="rId2"/>
+    <sheet name="ZY" sheetId="6" r:id="rId3"/>
+    <sheet name="Dash" sheetId="7" r:id="rId4"/>
+    <sheet name="PC" sheetId="8" r:id="rId5"/>
+    <sheet name="WH" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="51">
   <si>
     <t>Index</t>
   </si>
@@ -521,21 +526,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3B02F3-8668-4835-B18A-9EFEA275CE21}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="76.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="39.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="23.54296875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="76.81640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="39.7265625" style="6" customWidth="1"/>
     <col min="5" max="5" width="128" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="4"/>
+    <col min="6" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -552,7 +557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -569,7 +574,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
@@ -580,7 +585,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
@@ -591,7 +596,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
@@ -602,7 +607,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
@@ -613,7 +618,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
@@ -627,7 +632,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>23</v>
       </c>
@@ -638,7 +643,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>25</v>
       </c>
@@ -649,7 +654,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
         <v>28</v>
       </c>
@@ -660,7 +665,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
         <v>31</v>
       </c>
@@ -671,7 +676,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" s="4" t="s">
         <v>34</v>
       </c>
@@ -682,7 +687,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" s="4" t="s">
         <v>37</v>
       </c>
@@ -693,7 +698,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B14" s="4" t="s">
         <v>37</v>
       </c>
@@ -704,7 +709,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
         <v>42</v>
       </c>
@@ -715,7 +720,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B16" s="4" t="s">
         <v>45</v>
       </c>
@@ -726,7 +731,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>48</v>
       </c>
@@ -737,26 +742,192 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="D30" s="7"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="D31" s="7"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="D32" s="7"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D33" s="7"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D34" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F7DFCC-9BFD-4786-A850-EBDA07FF29AF}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="38.54296875" customWidth="1"/>
+    <col min="3" max="3" width="30.6328125" customWidth="1"/>
+    <col min="4" max="4" width="31.453125" customWidth="1"/>
+    <col min="5" max="5" width="32.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{231C8755-F20E-435C-A5DE-277B3102AC0A}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35FB229-AC04-413E-B2C6-DBCD16934489}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC661233-61AB-4A38-A0C4-60504A6FFE4A}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50B4F1B-824A-4176-9D3D-F97F6EFDA287}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update excel for bug data validation
</commit_message>
<xml_diff>
--- a/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test2/QuerySet2.xlsx
+++ b/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test2/QuerySet2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="709">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="710">
   <si>
     <t>Index</t>
   </si>
@@ -2146,19 +2146,28 @@
   </si>
   <si>
     <t>Select all while statements with s as control variable</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -2218,8 +2227,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2235,6 +2251,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE67C73"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF57BB8A"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2266,71 +2288,120 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF57BB8A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE67C73"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF57BB8A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE67C73"/>
+      <color rgb="FF57BB8A"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2607,8 +2678,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3B02F3-8668-4835-B18A-9EFEA275CE21}">
   <dimension ref="A1:G349"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="A215" sqref="A215:XFD215"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2616,7 +2689,7 @@
     <col min="1" max="1" width="6" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" style="5" customWidth="1"/>
     <col min="3" max="3" width="76.85546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="43.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="43.42578125" style="20" customWidth="1"/>
     <col min="5" max="5" width="74.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="47.28515625" style="5" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" style="5" customWidth="1"/>
@@ -2624,19 +2697,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="4" t="s">
@@ -2663,7 +2736,9 @@
         <v>128</v>
       </c>
       <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="G2" s="21" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
@@ -2682,7 +2757,7 @@
         <v>130</v>
       </c>
       <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
@@ -2701,7 +2776,7 @@
         <v>132</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
@@ -2720,7 +2795,7 @@
         <v>134</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
@@ -2739,7 +2814,7 @@
         <v>137</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
@@ -9011,6 +9086,19 @@
       <c r="G349" s="4"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"BUG"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G349" xr:uid="{A7AFEEE8-FE43-453E-9495-F53A09A6EB3D}">
+      <formula1>"PASS, BUG"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>